<commit_message>
data for 5 keV (#24)
</commit_message>
<xml_diff>
--- a/data/processed/spectra.xlsx
+++ b/data/processed/spectra.xlsx
@@ -7,9 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="12keV_0.5um" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="12keV_1.0um" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="12keV_2.0um" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="5keV_0.5um" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="12keV_0.5um" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="5keV_1.0um" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="12keV_1.0um" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="5keV_2.0um" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="12keV_2.0um" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,6 +430,705 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>fy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>yfy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ydy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fz</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>zfz</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>zdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.692781499446003</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.06450911332351555</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1091998335797128</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.02467181204681079</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.381309703547938</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.06450911332351555</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.08910706420104562</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.02221397771459845</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.082877735444422</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.07806572907455195</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1626013689906205</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.04520288385649351</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.699628232122648</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.07806572907455195</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.1326827170963463</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.04069972050364775</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.547478966804453</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.08229603901270859</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2096474284361938</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.07128174355669881</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.078742836912433</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.08229603901270859</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.1710723016039341</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.06418057416382247</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.077585052185827</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.09885846975166758</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.3042453487896969</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1249718442670211</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.511309402583635</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.09885846975166758</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.2482642046123926</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1125220052030484</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3.792238689061611</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1255096666970749</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.475962613899875</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.240905476548714</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.094466770274274</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1255096666970749</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.388385492942298</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.2169061955086356</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.365571919374333</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1347062589173376</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5880698612934976</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3426480282118973</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.562306686209455</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1347062589173376</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.479865006815494</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.3085130369917073</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4.99790898149042</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1256006206197993</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.627740469876466</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4187421112217966</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4.078293728896183</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1256006206197993</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.5122362234191963</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.3770265398097224</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5.876024209865426</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1089294647645549</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.6400721721242073</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5019849422253233</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.794835755250187</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1089294647645549</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.5222988924533531</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.4519766241125678</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>7.008384231226458</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.09373365944988575</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6569215008237301</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6144825404895702</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5.71884153268079</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.09373365944988575</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.5360479446721638</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.5532670820670279</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8.092408792572144</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.08152139297529248</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.6597044372959859</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.7125336612503221</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6.603405574738868</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.08152139297529248</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5383188208335244</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.6415502372458262</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>9.57000656926253</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.06554801149139393</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.6272949005747357</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8012391478493743</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7.809125360518224</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.06554801149139393</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5118726388689843</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.72141878110208</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11.67893651000781</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.04282548738196545</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.5001561481441151</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.779627368850448</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9.530012192166375</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.04282548738196545</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.4081274168855979</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.7019599924186993</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>12.44312334597123</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0345083564020353</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.429391735177261</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.7131177633854282</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10.15358865031252</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0345083564020353</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.350383655904645</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.6420761504534852</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>13.34567528603373</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0253463217893041</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.3382637802953739</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.6025238178287133</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10.89007103340352</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0253463217893041</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.2760232447210251</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.5424997011312739</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14.01363215024909</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.01975409763448841</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.2768266577098264</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.517769888589021</v>
+      </c>
+      <c r="F16" t="n">
+        <v>11.43512383460326</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.01975409763448841</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.2258905526912183</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.4661890559389783</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>14.53709226477959</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0160058284359973</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.2326782047483256</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.45145183078774</v>
+      </c>
+      <c r="F17" t="n">
+        <v>11.86226728806014</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0160058284359973</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.1898654150746336</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.4064776794386235</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>14.99263612519897</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.01259416027971168</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1888196623761514</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.3778360434765906</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12.23399107816236</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.01259416027971168</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.1540768444989395</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.3401955816474368</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>15.46245520689279</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.009533514933669501</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1474115476261082</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.3042202561654421</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12.61736344882452</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.009533514933669501</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.1202878228629043</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.2739134838562509</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>15.94652650731254</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.006848566021612694</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1092108396007268</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.2324395427686317</v>
+      </c>
+      <c r="F20" t="n">
+        <v>13.01236562996703</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.006848566021612694</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.08911604511419306</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2092836478024842</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>16.34746847313729</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.004608371143886555</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.07533520198720106</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.1643715433480053</v>
+      </c>
+      <c r="F21" t="n">
+        <v>13.33953427408002</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.004608371143886555</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.06147352482155607</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.1479966608824233</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>16.76046852738451</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.00237279465038678</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.03976915005975395</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.08896324827001179</v>
+      </c>
+      <c r="F22" t="n">
+        <v>13.67654231834576</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.00237279465038678</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.03245162644875923</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.08010062701267168</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>17.49054790713588</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0005086280148551654</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.008896182660735689</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.02076755040689138</v>
+      </c>
+      <c r="F23" t="n">
+        <v>14.27228709222288</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0005086280148551654</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.007259285051160322</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.01869866311603647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1642,7 +2344,938 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>fy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>yfy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ydy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fz</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>zfz</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>zdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9893259504956234</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1261171317624609</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1247709512546785</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.02668897448100394</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2018224939011072</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1261171317624609</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.02545327405595441</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.005517556037156677</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.235473706825951</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1483184544483554</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1832435507080057</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.04894870483628333</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.252036636192494</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1483184544483554</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.03738168434443315</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.01011943048140215</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.612666095585981</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1554417378141001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2506756204117646</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.08740485431440481</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.3289838834995402</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1554417378141001</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.05113782656399997</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01806967824644206</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2.193407838438227</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1454083358218283</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.3189397835658563</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.151254075560824</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.4474551990413982</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1454083358218283</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.06506371584743467</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.03126957307217539</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.760941577946453</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1419829353044777</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.3920065894410139</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2340073958681295</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5632320819010764</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1419829353044777</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.07996934424596683</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04837761453631329</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3.474092132729425</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1298249476289061</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.4510238291895923</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3387816031475288</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.7087147950768027</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1298249476289061</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.09200886115467682</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.07003815306034761</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3.965048298524905</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1242168742686704</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.4925259059670736</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4222372648885435</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.8088698528990806</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1242168742686704</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.100475284817283</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0872913933675683</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4.510778900410494</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1187079028904229</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5354651036700975</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.5222298749323806</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9201988956837407</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1187079028904229</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.1092348811486999</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1079634064346539</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5.145354651551323</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1119037713318665</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5757845903485551</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.6405519410458838</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.04965234891647</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1119037713318665</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.1174600564311052</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1324247670867119</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>5.648754141484325</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1073783183974501</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.6065537207532188</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.7407999479747085</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.152345844862802</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1073783183974501</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.1237369590336566</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1531495797331008</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6.03743305214536</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.1074407037075836</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.648666055709922</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8467447243102955</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.231636342637653</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1074407037075836</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.1323278753648241</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1750521163289409</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6.27612485585478</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.119643206435562</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.7508957017443956</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.018943709225917</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.280329470594375</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.119643206435562</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.1531827231558567</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2106517437889504</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6.374194376153932</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.132269130678617</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.8431091489104102</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.161951776102065</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.300335652735402</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.132269130678617</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.1719942663777237</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.240216574888632</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>6.469215354972919</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1490837312026252</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9644547630726782</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.349001616922409</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.319719932414475</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1490837312026252</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.1967487716668263</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.2788864001081082</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>6.563716609706894</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.1668724945199128</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.095303763983574</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.554402196886168</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.338998188380206</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1668724945199128</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.2234419678526491</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.321349972877499</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>6.608364363384986</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.1786117516055092</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.180331534191618</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.686463669497513</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.348106330130537</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1786117516055092</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.2407876329750901</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.3486517553420577</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>6.690948131238958</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.1897646972866494</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.269705746685233</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.836833315104775</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.364953418772747</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.1897646972866494</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.2590199723237876</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.3797384854266469</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>6.77176714963315</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.2030195554771665</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.374801156513401</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.012893995512818</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.381440498525162</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.2030195554771665</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.2804594359287337</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.4161364620811162</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>7.052247643602882</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.1755615077226089</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.238103229144138</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1.887832289378859</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.438658519294988</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1755615077226089</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.2525730587454041</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.390281779197453</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>7.417456914285767</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.1429355059362598</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.060217956803844</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.700314220936042</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.513161210514296</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1429355059362598</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.2162844631879842</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.3515151547492548</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>7.733343875484078</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.1164321188164802</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.900409612959062</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.505519706057104</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.577602150598752</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1164321188164802</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.1836835610436486</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.3112442311759163</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>7.940653413130647</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.09803583215435614</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.7784685652055914</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.336522641347691</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.619893296278652</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.09803583215435614</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.1588075873019406</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.2763065539971676</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>8.076487942082082</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.08539005806397756</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.6896517743274037</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.204290904146357</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.647603540184745</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.08539005806397756</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.1406889619627903</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.2489695718130738</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>8.225798810287404</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.06750967870071112</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.5553210347391945</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9876457668853114</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1.67806295729863</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.06750967870071112</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.1132854910867957</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.2041813508993733</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>8.348611318345016</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.05335527026195441</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.4454424132023099</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.804053243156162</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.703116708942383</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.05335527026195441</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0908702522932712</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.1662262755404608</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>8.466762171957553</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.04310969679556542</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.364999550073253</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.6681726411998925</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.727219483079341</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.04310969679556542</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.07445990821494361</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.1381349438113259</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>8.592665415960525</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.03058494372997412</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.2628061882376473</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.4882502652994267</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1.752903744855947</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.03058494372997412</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.05361246240048006</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.1009386179623964</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>8.745842093954588</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0188642686305392</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.1649839146606368</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.3119767541538954</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.784151787166736</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0188642686305392</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.03365671859076991</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0644966416585078</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>8.839159972303156</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.01216369855676736</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.1075168773981397</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.2054786179008392</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1.803188634349844</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.01216369855676736</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.02193344298922049</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.04247970597417793</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>8.938744854003575</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.003605035723825381</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.03222449452484318</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.06227900336095216</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1.823503950216729</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.003605035723825381</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.006573796883068008</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.01287527519001909</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2747,7 +4380,967 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>fy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>yfy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ydy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fz</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>zfz</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>zdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5817789302970161</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1167515839774646</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.06792361163689162</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.01398297945296711</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.02967072544514782</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1167515839774646</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.003464104193481472</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0007051767090371467</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7032977846908371</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1559862503003283</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1097047842784513</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0273014540477754</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.03586818701923269</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1559862503003283</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.005594943998201016</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.001376841722616841</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8861870499091471</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1649116906857514</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1461426046643358</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.04582718735312508</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0451955395453665</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1649116906857514</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.007453272837881127</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.002311114399531506</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.015476042380667</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1782296698000647</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1809879597233828</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.06503397901843844</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.051789278161414</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1782296698000647</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.009230385945892519</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.003279733582822501</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.17058886923052</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.169864687628734</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1988417126135152</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0823631306219097</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.05970003233075651</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.169864687628734</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.01014092734328927</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.004153661356173308</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1.397984399041081</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1650161877737657</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2306900560969581</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1141174766551298</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.07129720435109514</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1650161877737657</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.01176519286094486</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.00575506721596533</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1.708958028744181</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1658472577527584</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.283426002681782</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.17139259289914</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.08715685946595322</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1658472577527584</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.01445472613677088</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.008643512995244559</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2.003912359726757</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1650101012641617</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3306657814030176</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.2344708939186586</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1021995303460646</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1650101012641617</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.01686395485155389</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.01182461963093799</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2.28784593732461</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1607547279992458</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3677820513587972</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.2977407426019143</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1166801428035551</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1607547279992458</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.01875688461929866</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.01501538622154963</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2.673185578722337</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1572184917603947</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.4202742048823637</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3975418049820103</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1363324645148392</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.1572184917603947</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.02143398444900054</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.02004846125139768</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.984798653658629</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.1753273563524468</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.52331685719031</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.5527143308985893</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1522247313365901</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1753273563524468</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0266891597167058</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.02787397880485552</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3.112484100154514</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.2087881685958387</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6498498550549278</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.7157166631687542</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.1587366891078802</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.2087881685958387</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.03314234260780131</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.03609436192293723</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3.155716151898631</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.2738937023198486</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.8643307803140615</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.9651590170767115</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.1609415237468302</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.2738937023198486</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.04408086979601714</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.0486740084006389</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3.172931877908977</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.3832025340284216</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.215875535914279</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.365119998108172</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.1618195257733578</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3832025340284216</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0620096523316282</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.06884447130489395</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3.197894036642503</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.5486122634812605</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.754403885815669</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.985247282713119</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.1630925958687676</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.5486122634812605</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.08947459817659908</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.1001181579474833</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3.240745939258245</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.6590886268911155</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.135938791208675</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.449372001525287</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1652780429021705</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.6590886268911155</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.1089328783516424</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.1235244672319689</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3.26025205049962</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.7482948939608297</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.439629962414191</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.814466578184259</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.1662728545754806</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.7482948939608297</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.1244211280831237</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.141936579823685</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3.270000866201694</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.7923279850273388</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.590913197355241</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.997931403470915</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.1667700441762864</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.7923279850273388</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.1321365730651173</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.1511889084961888</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3.293798097434808</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.8076724564773631</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.660310000495636</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.100631693452795</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.1679837029691752</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.8076724564773631</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.1356758100252774</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.1563681946955414</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3.472413667729859</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.6922258327131292</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.403694442668753</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2.953463968051742</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.1770930970542228</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.6922258327131292</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.1225884165761064</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.1489463678507071</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>3.700429692684117</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.5549210916947316</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.05344648480387</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.688787662911584</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.18872191432689</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.5549210916947316</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.1047257707249974</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.1355984568102426</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.857494605252511</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.4402032175218639</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.698081536805388</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.317847335329607</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1967322248678781</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.4402032175218639</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.08660215837707476</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.1168915367054638</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>3.920865542631083</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.375471902456436</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.472174844567579</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.042501115883381</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1999641426741852</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.375471902456436</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.07508091707294652</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.1030055303984383</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>3.992644363040879</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.3256382100180858</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.300157563619432</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.836866422108384</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.2036248625150848</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.3256382100180858</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.06630803574459104</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.09263515138816635</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>4.070776843630131</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.2650451071238873</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.078939484597388</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.554158623931043</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.2076096190251367</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.2650451071238873</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.05502591371446679</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.07837789273965047</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4.136187390774192</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.2148821149597843</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.8887926943995501</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.300833291456915</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.2109455569294838</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.2148821149597843</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.04532842741437705</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.06560242347212322</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>4.218124051143658</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.1593800191774348</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.672284692164075</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1.003444901964842</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.2151243266083265</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.1593800191774348</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.03428651930036782</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.05060480679727517</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4.298639915685178</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.1147189276297737</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.4931353613939443</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.7500982864169656</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.2192306356999441</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.1147189276297737</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.02514990343109116</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.03782826420142368</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>4.353998891279449</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.07570056322762914</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.3296001683623271</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.5078046805026357</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.2220539434552519</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.07570056322762914</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.01680960858647868</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.02560913678196982</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>4.435014920903419</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0407784499235419</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.1808530338622212</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.2838192475842236</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.2261857609660744</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.0407784499235419</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.009223504726973281</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.01431331023878267</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>4.493720362293042</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.002729653021518283</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01226629736479143</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.01950475469779578</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.2291797384769451</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.002729653021518283</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.000625581165604363</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.0009836457798305537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>